<commit_message>
feat: isCalculate 為 true 建立全新的幣別設定EXCEL與SQL腳本
</commit_message>
<xml_diff>
--- a/input/匯率表.xlsx
+++ b/input/匯率表.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\chiisen\min_bet.ts\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3538BA93-04A8-480F-A3F7-071B0194332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC271BC-368E-480E-8566-39313BCB7661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="匯率表" sheetId="1" r:id="rId1"/>
+    <sheet name="匯率表" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">匯率表!$A$1:$C$21</definedName>
-  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>幣別</t>
   </si>
@@ -39,124 +36,22 @@
     <t>匯率名稱</t>
   </si>
   <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>SAR</t>
-  </si>
-  <si>
-    <t>AED</t>
-  </si>
-  <si>
-    <t>NIO</t>
-  </si>
-  <si>
-    <t>ARS</t>
-  </si>
-  <si>
-    <t>DKK</t>
-  </si>
-  <si>
-    <t>DOP</t>
-  </si>
-  <si>
-    <t>ILS</t>
-  </si>
-  <si>
-    <t>MOP</t>
-  </si>
-  <si>
-    <t>VEF</t>
-  </si>
-  <si>
-    <t>COP</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>PYG</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
-    <t>BOB</t>
-  </si>
-  <si>
-    <t>DZD</t>
-  </si>
-  <si>
-    <t>CLP</t>
-  </si>
-  <si>
-    <t>VES</t>
-  </si>
-  <si>
-    <t>LRD</t>
-  </si>
-  <si>
-    <t>BZD</t>
-  </si>
-  <si>
-    <t>亞美尼亞德拉姆</t>
-  </si>
-  <si>
-    <t>阿根廷披索</t>
-  </si>
-  <si>
-    <t>阿聯酋迪拉姆</t>
-  </si>
-  <si>
-    <t>玻利維亞玻利維亞諾</t>
-  </si>
-  <si>
-    <t>伯利茲元</t>
-  </si>
-  <si>
-    <t>智利披索</t>
-  </si>
-  <si>
-    <t>哥倫比亞披索</t>
-  </si>
-  <si>
-    <t>丹麥克朗</t>
-  </si>
-  <si>
-    <t>多米尼加披索</t>
-  </si>
-  <si>
-    <t>阿爾及利亞第納爾</t>
-  </si>
-  <si>
-    <t>英鎊</t>
-  </si>
-  <si>
-    <t>以色列謝克爾</t>
-  </si>
-  <si>
-    <t>利比里亞元</t>
-  </si>
-  <si>
-    <t>摩洛哥迪拉姆</t>
-  </si>
-  <si>
-    <t>澳門幣</t>
-  </si>
-  <si>
-    <t>尼加拉瓜科多巴</t>
-  </si>
-  <si>
-    <t>巴拉圭瓜拉尼</t>
-  </si>
-  <si>
-    <t>沙地阿拉伯利雅</t>
-  </si>
-  <si>
-    <t>委內瑞拉玻利瓦</t>
-  </si>
-  <si>
-    <t>委內瑞拉玻利瓦爾</t>
+    <t>ZWD</t>
+  </si>
+  <si>
+    <t>津巴布韋元</t>
+  </si>
+  <si>
+    <t>納米比亞元</t>
+  </si>
+  <si>
+    <t>阿里亞里</t>
+  </si>
+  <si>
+    <t>MGA</t>
+  </si>
+  <si>
+    <t>NAD</t>
   </si>
 </sst>
 </file>
@@ -233,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,9 +137,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -560,19 +452,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69411EED-BCB2-4108-BF28-62747F6952D5}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20:C21"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,24 +480,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>0.54857299999999998</v>
+        <v>51.2241</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>61.129322999999999</v>
+        <v>2.4186899999999998</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,211 +505,15 @@
         <v>7</v>
       </c>
       <c r="B4" s="3">
-        <v>18.677599000000001</v>
+        <v>612.75199999999995</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3">
-        <v>138.42153999999999</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3">
-        <v>615.07879000000003</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1.0631299999999999</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>8.160482</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
-        <v>21.899182</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0.12310400000000001</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.51782700000000004</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3">
-        <v>22.67</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1.5166040000000001</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.207489</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B17" s="3">
-        <v>5.3725120000000004</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
-        <v>1030.8399999999999</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0.56017700000000004</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="4">
-        <v>82215.929999999993</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="3">
-        <v>0.82215899999999997</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C21" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C21">
-      <sortCondition ref="A1:A21"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;Kffffff頁 &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>